<commit_message>
Commit on 31-Oct-2022 5:29 PM
</commit_message>
<xml_diff>
--- a/src/main/java/com/flipcart/testdata/Controller.xlsx
+++ b/src/main/java/com/flipcart/testdata/Controller.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{E8B4BFED-8D32-4763-AAE6-FB2378C106C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BDC9ADF-891E-4BE5-88C2-E79AE51D3D64}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{E8B4BFED-8D32-4763-AAE6-FB2378C106C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{929284ED-3036-4AA8-B4E9-9B96A81C1430}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,13 +40,13 @@
     <t>Dress</t>
   </si>
   <si>
-    <t>Printed</t>
-  </si>
-  <si>
     <t>Summer</t>
   </si>
   <si>
     <t>Faded</t>
+  </si>
+  <si>
+    <t>Pant</t>
   </si>
 </sst>
 </file>
@@ -367,7 +367,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -389,7 +389,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -397,7 +397,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -405,7 +405,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -413,7 +413,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>